<commit_message>
config cors and trustProxy
</commit_message>
<xml_diff>
--- a/Thống kê theo học kỳ.xlsx
+++ b/Thống kê theo học kỳ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Năm học</t>
   </si>
@@ -22,12 +22,6 @@
     <t>Học kỳ</t>
   </si>
   <si>
-    <t>Ngày bắt đầu</t>
-  </si>
-  <si>
-    <t>Ngày kết thúc</t>
-  </si>
-  <si>
     <t>Tổng số môn học</t>
   </si>
   <si>
@@ -35,15 +29,6 @@
   </si>
   <si>
     <t>2023-2024</t>
-  </si>
-  <si>
-    <t>HK1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>HK2</t>
   </si>
 </sst>
 </file>
@@ -366,50 +351,32 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>

</xml_diff>